<commit_message>
seperate data into tables
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\auto_make_invoice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hengh\OneDrive\Desktop\auto_make_invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F8CE23-D355-4628-A679-EBBBDE2E7FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8582E8AE-606E-4E93-8995-AF5CAEFD0B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="给徐燕打印" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="62">
   <si>
     <t>货物装运通知单</t>
   </si>
@@ -79,9 +79,6 @@
     <t>级别</t>
   </si>
   <si>
-    <t>张数</t>
-  </si>
-  <si>
     <t>尺数</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>手册号</t>
   </si>
   <si>
-    <t>备注</t>
-  </si>
-  <si>
     <t>价格</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
     <t>A级</t>
   </si>
   <si>
-    <t>越南QC带走的</t>
-  </si>
-  <si>
     <t>VPL24B00440</t>
   </si>
   <si>
@@ -227,6 +218,12 @@
   </si>
   <si>
     <t>net</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>cbm</t>
   </si>
 </sst>
 </file>
@@ -234,8 +231,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="169" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="165" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -386,7 +383,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -398,7 +395,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -428,31 +425,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -770,32 +767,32 @@
   </sheetPr>
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" customWidth="1"/>
+    <col min="3" max="3" width="13.53515625" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="17.3828125" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" customWidth="1"/>
-    <col min="12" max="13" width="8.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.69140625" customWidth="1"/>
+    <col min="10" max="10" width="14.53515625" customWidth="1"/>
+    <col min="11" max="11" width="7.3828125" customWidth="1"/>
+    <col min="12" max="13" width="8.15234375" customWidth="1"/>
+    <col min="14" max="14" width="14.53515625" customWidth="1"/>
+    <col min="15" max="15" width="17.3046875" customWidth="1"/>
+    <col min="16" max="16" width="18.53515625" customWidth="1"/>
+    <col min="17" max="17" width="13.3046875" customWidth="1"/>
+    <col min="18" max="18" width="10.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="29.25">
+    <row r="1" spans="1:19" ht="28.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -818,7 +815,7 @@
       <c r="R1" s="17"/>
       <c r="S1" s="18"/>
     </row>
-    <row r="2" spans="1:19" ht="18">
+    <row r="2" spans="1:19" ht="17.149999999999999">
       <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
@@ -847,7 +844,7 @@
       </c>
       <c r="S2" s="18"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15.9">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -873,59 +870,59 @@
         <v>12</v>
       </c>
       <c r="I3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="L3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="P3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="Q3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="R3" s="19"/>
       <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75">
+    <row r="4" spans="1:19" ht="15.9">
       <c r="A4" s="6">
         <v>45636</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="I4" s="13">
         <v>190</v>
@@ -943,10 +940,10 @@
         <v>918</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P4" s="7">
         <v>1.1000000000000001</v>
@@ -959,30 +956,30 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75">
+    <row r="5" spans="1:19" ht="15.9">
       <c r="A5" s="6">
         <v>45636</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="I5" s="13">
         <v>190</v>
@@ -1000,11 +997,11 @@
         <v>916</v>
       </c>
       <c r="N5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="P5" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1014,30 +1011,30 @@
       </c>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75">
+    <row r="6" spans="1:19" ht="15.9">
       <c r="A6" s="6">
         <v>45636</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="I6" s="13">
         <v>190</v>
@@ -1055,11 +1052,11 @@
         <v>917.5</v>
       </c>
       <c r="N6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="P6" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1069,30 +1066,30 @@
       </c>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:19" ht="15.75">
+    <row r="7" spans="1:19" ht="15.9">
       <c r="A7" s="6">
         <v>45636</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="I7" s="13">
         <v>188</v>
@@ -1110,10 +1107,10 @@
         <v>957.5</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P7" s="7">
         <v>1.1000000000000001</v>
@@ -1124,30 +1121,30 @@
       </c>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:19" ht="15.75">
+    <row r="8" spans="1:19" ht="15.9">
       <c r="A8" s="6">
         <v>45637</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="I8" s="13">
         <v>190</v>
@@ -1165,10 +1162,10 @@
         <v>941</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P8" s="7">
         <v>1.1000000000000001</v>
@@ -1179,30 +1176,30 @@
       </c>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75">
+    <row r="9" spans="1:19" ht="15.9">
       <c r="A9" s="6">
         <v>45637</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I9" s="13">
         <v>200</v>
@@ -1220,10 +1217,10 @@
         <v>904</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P9" s="7">
         <v>1.1000000000000001</v>
@@ -1234,30 +1231,30 @@
       </c>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:19" ht="15.75">
+    <row r="10" spans="1:19" ht="15.9">
       <c r="A10" s="6">
         <v>45637</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G10" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I10" s="13">
         <v>210</v>
@@ -1275,10 +1272,10 @@
         <v>920</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P10" s="7">
         <v>1.1000000000000001</v>
@@ -1289,30 +1286,30 @@
       </c>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75">
+    <row r="11" spans="1:19" ht="15.9">
       <c r="A11" s="6">
         <v>45637</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G11" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" s="13">
         <v>115</v>
@@ -1330,10 +1327,10 @@
         <v>760</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P11" s="7">
         <v>1.1000000000000001</v>
@@ -1344,30 +1341,30 @@
       </c>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.9">
       <c r="A12" s="6">
         <v>45637</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="I12" s="13">
         <v>42</v>
@@ -1379,7 +1376,7 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="7">
@@ -1391,30 +1388,30 @@
       </c>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.9">
       <c r="A13" s="6">
         <v>45637</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G13" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" s="13">
         <v>8</v>
@@ -1426,7 +1423,7 @@
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
       <c r="N13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="7">
@@ -1438,33 +1435,33 @@
       </c>
       <c r="R13" s="8"/>
       <c r="S13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.9">
       <c r="A14" s="6">
         <v>45637</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G14" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I14" s="13">
         <v>147</v>
@@ -1482,10 +1479,10 @@
         <v>651</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P14" s="7">
         <v>1.1000000000000001</v>
@@ -1496,30 +1493,30 @@
       </c>
       <c r="R14" s="8"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75">
+    <row r="15" spans="1:19" ht="15.9">
       <c r="A15" s="6">
         <v>45637</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G15" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I15" s="13">
         <v>9</v>
@@ -1531,7 +1528,7 @@
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
       <c r="N15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="7">
@@ -1543,33 +1540,33 @@
       </c>
       <c r="R15" s="8"/>
       <c r="S15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.9">
       <c r="A16" s="6">
         <v>45638</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="G16" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I16" s="13">
         <v>85</v>
@@ -1587,10 +1584,10 @@
         <v>914</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P16" s="7">
         <v>1.57</v>
@@ -1603,77 +1600,84 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75">
-      <c r="A17" s="6">
-        <v>45638</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="13">
-        <v>115</v>
-      </c>
-      <c r="J17" s="13">
-        <v>5858.5</v>
-      </c>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
+    <row r="17" spans="1:19" ht="15.9">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="N17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="7">
-        <v>1.57</v>
-      </c>
-      <c r="Q17" s="8">
-        <f t="shared" si="0"/>
-        <v>9197.85</v>
-      </c>
-      <c r="R17" s="8"/>
-    </row>
-    <row r="18" spans="1:19" ht="15.75">
+        <v>15</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R17" s="19"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.9">
       <c r="A18" s="6">
         <v>45638</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="E18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="G18" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I18" s="13">
         <v>17</v>
@@ -1685,7 +1689,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="7">
@@ -1697,30 +1701,30 @@
       </c>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75">
+    <row r="19" spans="1:19" ht="15.9">
       <c r="A19" s="6">
         <v>45638</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="G19" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
@@ -1732,7 +1736,7 @@
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="7">
@@ -1744,33 +1748,33 @@
       </c>
       <c r="R19" s="8"/>
       <c r="S19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15.9">
       <c r="A20" s="6">
         <v>45638</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="G20" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I20" s="13">
         <v>103</v>
@@ -1788,10 +1792,10 @@
         <v>738</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P20" s="7">
         <v>1.1000000000000001</v>
@@ -1804,30 +1808,30 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15.75">
+    <row r="21" spans="1:19" ht="15.9">
       <c r="A21" s="6">
         <v>45638</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="G21" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I21" s="13">
         <v>51</v>
@@ -1839,7 +1843,7 @@
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="N21" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="7">
@@ -1851,30 +1855,30 @@
       </c>
       <c r="R21" s="8"/>
     </row>
-    <row r="22" spans="1:19" ht="15.75">
+    <row r="22" spans="1:19" ht="15.9">
       <c r="A22" s="6">
         <v>45638</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="E22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="G22" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I22" s="13">
         <v>15</v>
@@ -1886,7 +1890,7 @@
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
       <c r="N22" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="7">
@@ -1898,30 +1902,30 @@
       </c>
       <c r="R22" s="8"/>
     </row>
-    <row r="23" spans="1:19" ht="15.75">
+    <row r="23" spans="1:19" ht="15.9">
       <c r="A23" s="10">
         <v>45638</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="E23" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
@@ -1937,11 +1941,9 @@
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="O23" s="5"/>
       <c r="P23" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1952,30 +1954,30 @@
       <c r="R23" s="8"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" ht="15.75">
+    <row r="24" spans="1:19" ht="15.9">
       <c r="A24" s="6">
         <v>45636</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I24" s="13">
         <v>185</v>
@@ -1993,10 +1995,10 @@
         <v>893</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P24" s="7">
         <v>1.1000000000000001</v>
@@ -2009,30 +2011,30 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15.75">
+    <row r="25" spans="1:19" ht="15.9">
       <c r="A25" s="6">
         <v>45636</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G25" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I25" s="13">
         <v>185</v>
@@ -2050,10 +2052,10 @@
         <v>912</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P25" s="7">
         <v>1.1000000000000001</v>
@@ -2064,30 +2066,30 @@
       </c>
       <c r="R25" s="8"/>
     </row>
-    <row r="26" spans="1:19" ht="15.75">
+    <row r="26" spans="1:19" ht="15.9">
       <c r="A26" s="6">
         <v>45636</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G26" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I26" s="13">
         <v>106</v>
@@ -2105,10 +2107,10 @@
         <v>825.5</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P26" s="7">
         <v>1.1000000000000001</v>
@@ -2119,30 +2121,30 @@
       </c>
       <c r="R26" s="8"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75">
+    <row r="27" spans="1:19" ht="15.9">
       <c r="A27" s="6">
         <v>45636</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G27" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I27" s="13">
         <v>73</v>
@@ -2154,7 +2156,7 @@
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
       <c r="N27" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="7">
@@ -2166,30 +2168,30 @@
       </c>
       <c r="R27" s="8"/>
     </row>
-    <row r="28" spans="1:19" ht="15.75">
+    <row r="28" spans="1:19" ht="15.9">
       <c r="A28" s="6">
         <v>45636</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G28" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I28" s="13">
         <v>2</v>
@@ -2201,7 +2203,7 @@
       <c r="L28" s="22"/>
       <c r="M28" s="22"/>
       <c r="N28" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="7">
@@ -2213,33 +2215,33 @@
       </c>
       <c r="R28" s="8"/>
       <c r="S28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="15.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="15.9">
       <c r="A29" s="6">
         <v>45636</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G29" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I29" s="13">
         <v>135</v>
@@ -2257,10 +2259,10 @@
         <v>618.5</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P29" s="7">
         <v>1.1000000000000001</v>
@@ -2271,30 +2273,30 @@
       </c>
       <c r="R29" s="8"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75">
+    <row r="30" spans="1:19" ht="15.9">
       <c r="A30" s="6">
         <v>45636</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G30" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I30" s="13">
         <v>115</v>
@@ -2312,10 +2314,10 @@
         <v>544.5</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P30" s="7">
         <v>1.1000000000000001</v>
@@ -2326,30 +2328,30 @@
       </c>
       <c r="R30" s="8"/>
     </row>
-    <row r="31" spans="1:19" ht="15.75">
+    <row r="31" spans="1:19" ht="15.9">
       <c r="A31" s="6">
         <v>45638</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I31" s="13">
         <v>149</v>
@@ -2367,10 +2369,10 @@
         <v>930.5</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P31" s="7">
         <v>1.1000000000000001</v>
@@ -2381,30 +2383,30 @@
       </c>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:19" ht="15.75">
+    <row r="32" spans="1:19" ht="15.9">
       <c r="A32" s="6">
         <v>45638</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I32" s="13">
         <v>45</v>
@@ -2416,7 +2418,7 @@
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
       <c r="N32" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="7">
@@ -2428,30 +2430,30 @@
       </c>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:19" ht="15.75">
+    <row r="33" spans="1:19" ht="15.9">
       <c r="A33" s="6">
         <v>45638</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I33" s="13">
         <v>23</v>
@@ -2469,10 +2471,10 @@
         <v>463</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P33" s="7">
         <v>1.1000000000000001</v>
@@ -2483,30 +2485,30 @@
       </c>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:19" ht="15.75">
+    <row r="34" spans="1:19" ht="15.9">
       <c r="A34" s="6">
         <v>45638</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G34" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I34" s="13">
         <v>57</v>
@@ -2518,7 +2520,7 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="7">
@@ -2530,30 +2532,30 @@
       </c>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:19" ht="15.75">
+    <row r="35" spans="1:19" ht="15.9">
       <c r="A35" s="6">
         <v>45638</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G35" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I35" s="13">
         <v>1</v>
@@ -2565,7 +2567,7 @@
       <c r="L35" s="21"/>
       <c r="M35" s="21"/>
       <c r="N35" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="7">
@@ -2577,33 +2579,33 @@
       </c>
       <c r="R35" s="8"/>
       <c r="S35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="15.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="15.9">
       <c r="A36" s="6">
         <v>45638</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I36" s="13">
         <v>24</v>
@@ -2615,7 +2617,7 @@
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O36" s="4"/>
       <c r="P36" s="7">
@@ -2627,30 +2629,30 @@
       </c>
       <c r="R36" s="8"/>
     </row>
-    <row r="37" spans="1:19" ht="15.75">
+    <row r="37" spans="1:19" ht="15.9">
       <c r="A37" s="6">
         <v>45638</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I37" s="13">
         <v>1</v>
@@ -2662,7 +2664,7 @@
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O37" s="4"/>
       <c r="P37" s="7">
@@ -2674,7 +2676,7 @@
       </c>
       <c r="R37" s="8"/>
       <c r="S37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -2686,11 +2688,11 @@
       <c r="H38" s="1"/>
       <c r="I38">
         <f t="shared" ref="I38:M38" si="1">SUM(I4:I37)</f>
-        <v>3168</v>
+        <v>3053</v>
       </c>
       <c r="J38">
         <f t="shared" si="1"/>
-        <v>165080.79999999996</v>
+        <v>159222.29999999999</v>
       </c>
       <c r="K38" s="1">
         <f t="shared" si="1"/>
@@ -2707,11 +2709,11 @@
       <c r="O38" s="16"/>
       <c r="P38" s="1">
         <f>SUM(P4:P37)</f>
-        <v>39.280000000000022</v>
+        <v>37.710000000000022</v>
       </c>
       <c r="Q38">
         <f>SUM(Q4:Q37)</f>
-        <v>186897.91999999998</v>
+        <v>177700.06999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2729,7 +2731,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2745,7 +2747,7 @@
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>